<commit_message>
add upload file logic on vehicles and employees
</commit_message>
<xml_diff>
--- a/static/templates/employeesTemplate.xlsx
+++ b/static/templates/employeesTemplate.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26424"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAF68DFD-1DA7-45F6-9B2F-6B811E0E11F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91528D8A-5B58-42A0-9C0A-CE66BE96088A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="Entities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -507,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>

</xml_diff>